<commit_message>
localization work but there is a fix to do with some sign in the wall
</commit_message>
<xml_diff>
--- a/camera_data.xlsx
+++ b/camera_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\Desktop\SensorFusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2463655E-FAB6-4FCA-9C42-A04E71257370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A229D0C-FC7B-4615-A579-373ECCCF516A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{6EA62ED9-EE76-41B3-B6EF-A5DE8522FDB5}"/>
   </bookViews>
@@ -33,6 +33,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
+    <t xml:space="preserve">wood </t>
+  </si>
+  <si>
     <t>fixed_camera_distance</t>
   </si>
   <si>
@@ -42,10 +45,7 @@
     <t>our measurement  cm</t>
   </si>
   <si>
-    <t>green piece (cm)</t>
-  </si>
-  <si>
-    <t>wood  (cm)</t>
+    <t>pcb (cm)</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="B1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D3" sqref="D3:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,13 +413,13 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1">
         <v>1.4</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E1">
         <v>5</v>
@@ -427,13 +427,13 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">

</xml_diff>